<commit_message>
Final commit from virtusa
</commit_message>
<xml_diff>
--- a/res/input/testReadExcel.xlsx
+++ b/res/input/testReadExcel.xlsx
@@ -2,21 +2,41 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" date1904="false" showObjects="all"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="500" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Department" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Department" r:id="rId2" sheetId="1" state="visible"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr iterate="false" iterateCount="100" iterateDelta="0.0001" refMode="A1"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -57,7 +77,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border diagonalDown="false" diagonalUp="false">
       <left/>
       <right/>
       <top/>
@@ -66,43 +86,43 @@
     </border>
   </borders>
   <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
+    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
+    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
+    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
+    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
+    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -112,20 +132,46 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A2:B6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="1:1048576"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A3" activeCellId="0" pane="topLeft" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.6632653061225"/>
+    <col min="1" max="1025" hidden="false" style="0" width="10.3928571428571" collapsed="true"/>
   </cols>
-  <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <sheetData>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>